<commit_message>
adl2 reste invaincu !
</commit_message>
<xml_diff>
--- a/Championnat.xlsx
+++ b/Championnat.xlsx
@@ -203,13 +203,14 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -493,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S44"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,12 +681,12 @@
       <c r="E7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>16</v>
+      <c r="F7" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="G7" s="1"/>
       <c r="Q7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R7">
         <v>1</v>
@@ -782,8 +783,8 @@
       <c r="F10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>9</v>
+      <c r="G10" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>7</v>
@@ -793,10 +794,10 @@
       </c>
       <c r="J10" s="1"/>
       <c r="Q10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S10" t="s">
         <v>9</v>
@@ -821,8 +822,8 @@
       <c r="F11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>10</v>
+      <c r="G11" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>10</v>
@@ -835,10 +836,10 @@
       </c>
       <c r="K11" s="1"/>
       <c r="Q11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S11" t="s">
         <v>10</v>
@@ -1116,10 +1117,10 @@
         <v>5</v>
       </c>
       <c r="F18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G18">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -1163,10 +1164,10 @@
         <v>5</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>6</v>
@@ -1218,12 +1219,6 @@
       <c r="H29" t="s">
         <v>31</v>
       </c>
-      <c r="M29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N29" s="2">
-        <v>9</v>
-      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
@@ -1245,7 +1240,7 @@
         <v>6</v>
       </c>
       <c r="N30" s="2">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -1288,7 +1283,7 @@
         <v>12</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="N32" s="2">
         <v>8</v>
@@ -1310,11 +1305,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M33" t="s">
-        <v>10</v>
-      </c>
-      <c r="N33">
-        <v>7</v>
+      <c r="M33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N33" s="2">
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="5:14" x14ac:dyDescent="0.25">
@@ -1323,20 +1318,20 @@
       </c>
       <c r="F34" s="2">
         <f>F18+Q6</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G34">
         <f>F19+R6</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H34">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M34" t="s">
-        <v>11</v>
-      </c>
-      <c r="N34">
+      <c r="M34" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N34" s="6">
         <v>7</v>
       </c>
     </row>
@@ -1346,20 +1341,20 @@
       </c>
       <c r="F35" s="2">
         <f>G18+Q7</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G35">
         <f>G19+R7</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="M35" t="s">
-        <v>12</v>
-      </c>
-      <c r="N35">
+        <v>13</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N35" s="6">
         <v>7</v>
       </c>
     </row>
@@ -1379,10 +1374,10 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M36" t="s">
-        <v>2</v>
-      </c>
-      <c r="N36">
+      <c r="M36" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N36" s="6">
         <v>7</v>
       </c>
     </row>
@@ -1402,10 +1397,10 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="M37" t="s">
-        <v>3</v>
-      </c>
-      <c r="N37">
+      <c r="M37" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N37" s="6">
         <v>6</v>
       </c>
     </row>
@@ -1415,20 +1410,20 @@
       </c>
       <c r="F38">
         <f>J18+Q10</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G38">
         <f>J19+R10</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H38">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="M38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N38">
+      <c r="M38" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N38" s="6">
         <v>6</v>
       </c>
     </row>
@@ -1438,21 +1433,21 @@
       </c>
       <c r="F39">
         <f>K18+Q11</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G39">
         <f>K19+R11</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H39">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="M39" t="s">
-        <v>1</v>
-      </c>
-      <c r="N39">
-        <v>4</v>
+      <c r="M39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N39" s="6">
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="5:14" x14ac:dyDescent="0.25">
@@ -1471,10 +1466,10 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="M40" t="s">
-        <v>8</v>
-      </c>
-      <c r="N40">
+      <c r="M40" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N40" s="6">
         <v>4</v>
       </c>
     </row>
@@ -1494,11 +1489,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="M41" t="s">
-        <v>9</v>
-      </c>
-      <c r="N41">
-        <v>3</v>
+      <c r="M41" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N41" s="6">
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="5:14" x14ac:dyDescent="0.25">
@@ -1515,11 +1510,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M42" t="s">
-        <v>7</v>
-      </c>
-      <c r="N42">
-        <v>1</v>
+      <c r="M42" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N42" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="5:14" x14ac:dyDescent="0.25">
@@ -1538,11 +1533,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="M43" t="s">
-        <v>13</v>
-      </c>
-      <c r="N43">
-        <v>0</v>
+      <c r="M43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N43" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="5:14" x14ac:dyDescent="0.25">
@@ -1561,10 +1556,20 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="M44" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N44" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
     </row>
   </sheetData>
-  <sortState ref="M29:N43">
-    <sortCondition descending="1" ref="N43"/>
+  <sortState ref="M30:N44">
+    <sortCondition descending="1" ref="N30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
évaluation : 5 champion selectionnés
</commit_message>
<xml_diff>
--- a/Championnat.xlsx
+++ b/Championnat.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Resultat nom" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="39">
   <si>
     <t>Algo/Alog</t>
   </si>
@@ -124,13 +125,25 @@
   </si>
   <si>
     <t>ald12</t>
+  </si>
+  <si>
+    <t>adl</t>
+  </si>
+  <si>
+    <t>adlKiller</t>
+  </si>
+  <si>
+    <t>adlKILLER</t>
+  </si>
+  <si>
+    <t>adlkiller</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,8 +180,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +217,12 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -212,7 +239,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -220,6 +247,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -503,20 +532,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" customWidth="1"/>
+    <col min="13" max="14" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" customWidth="1"/>
+    <col min="17" max="18" width="9" customWidth="1"/>
+    <col min="19" max="19" width="15" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -565,29 +608,35 @@
       <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="R2">
-        <v>0</v>
-      </c>
       <c r="S2">
         <v>0</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -595,17 +644,17 @@
         <v>14</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="R3">
+      <c r="S3">
         <v>0</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>1</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -616,17 +665,17 @@
         <v>17</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="R4">
-        <v>1</v>
-      </c>
       <c r="S4">
         <v>1</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -640,17 +689,17 @@
         <v>15</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="R5">
+      <c r="S5">
         <v>0</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>2</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -667,17 +716,17 @@
         <v>4</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="R6">
-        <v>2</v>
-      </c>
       <c r="S6">
         <v>2</v>
       </c>
-      <c r="T6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T6">
+        <v>2</v>
+      </c>
+      <c r="U6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -697,50 +746,50 @@
         <v>21</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="R7">
+      <c r="S7">
         <v>1</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>3</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>21</v>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="R8">
-        <v>1</v>
-      </c>
       <c r="S8">
-        <v>3</v>
-      </c>
-      <c r="T8" t="s">
+        <v>6</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -763,20 +812,20 @@
         <v>31</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="R9">
+      <c r="S9">
         <v>1</v>
       </c>
-      <c r="S9">
-        <v>5</v>
-      </c>
-      <c r="T9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T9">
+        <v>5</v>
+      </c>
+      <c r="U9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -796,26 +845,26 @@
         <v>5</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="R10">
-        <v>2</v>
-      </c>
       <c r="S10">
-        <v>5</v>
-      </c>
-      <c r="T10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="T10">
+        <v>5</v>
+      </c>
+      <c r="U10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -837,8 +886,8 @@
       <c r="G11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>8</v>
+      <c r="H11" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>6</v>
@@ -847,17 +896,17 @@
         <v>7</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="R11">
-        <v>5</v>
-      </c>
       <c r="S11">
         <v>4</v>
       </c>
-      <c r="T11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T11">
+        <v>5</v>
+      </c>
+      <c r="U11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -880,7 +929,7 @@
         <v>9</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>9</v>
@@ -892,17 +941,17 @@
         <v>9</v>
       </c>
       <c r="L12" s="1"/>
-      <c r="R12">
-        <v>6</v>
-      </c>
       <c r="S12">
+        <v>6</v>
+      </c>
+      <c r="T12">
         <v>4</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -925,7 +974,7 @@
         <v>31</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>22</v>
@@ -940,17 +989,17 @@
         <v>22</v>
       </c>
       <c r="M13" s="1"/>
-      <c r="R13">
-        <v>6</v>
-      </c>
       <c r="S13">
-        <v>5</v>
-      </c>
-      <c r="T13" t="s">
+        <v>6</v>
+      </c>
+      <c r="T13">
+        <v>5</v>
+      </c>
+      <c r="U13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -972,8 +1021,8 @@
       <c r="G14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>34</v>
+      <c r="H14" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>11</v>
@@ -991,17 +1040,17 @@
         <v>11</v>
       </c>
       <c r="N14" s="1"/>
-      <c r="R14">
-        <v>5</v>
-      </c>
       <c r="S14">
-        <v>7</v>
-      </c>
-      <c r="T14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T14">
+        <v>6</v>
+      </c>
+      <c r="U14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1045,17 +1094,17 @@
         <v>16</v>
       </c>
       <c r="O15" s="1"/>
-      <c r="R15">
-        <v>0</v>
-      </c>
       <c r="S15">
         <v>0</v>
       </c>
-      <c r="T15" t="s">
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1075,10 +1124,10 @@
         <v>5</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>13</v>
@@ -1102,17 +1151,17 @@
         <v>16</v>
       </c>
       <c r="P16" s="1"/>
-      <c r="R16">
-        <v>8</v>
-      </c>
       <c r="S16">
-        <v>5</v>
-      </c>
-      <c r="T16" t="s">
+        <v>8</v>
+      </c>
+      <c r="T16">
+        <v>5</v>
+      </c>
+      <c r="U16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1132,10 +1181,10 @@
         <v>5</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>20</v>
@@ -1146,7 +1195,7 @@
       <c r="K17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="L17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="M17" s="4" t="s">
@@ -1162,512 +1211,718 @@
         <v>20</v>
       </c>
       <c r="Q17" s="1"/>
-      <c r="R17">
-        <v>8</v>
-      </c>
       <c r="S17">
-        <v>5</v>
-      </c>
-      <c r="T17" t="s">
+        <v>8</v>
+      </c>
+      <c r="T17">
+        <v>5</v>
+      </c>
+      <c r="U17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R18" s="1"/>
+      <c r="S18">
+        <v>15</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B19">
-        <v>7</v>
-      </c>
-      <c r="C19">
-        <v>8</v>
-      </c>
-      <c r="D19">
-        <v>6</v>
-      </c>
-      <c r="E19">
-        <v>8</v>
-      </c>
-      <c r="F19">
-        <v>6</v>
-      </c>
-      <c r="G19">
-        <v>6</v>
-      </c>
-      <c r="H19">
-        <v>7</v>
-      </c>
-      <c r="I19">
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="I20">
         <v>1</v>
       </c>
-      <c r="J19">
+      <c r="J20">
         <v>2</v>
       </c>
-      <c r="K19">
+      <c r="K20">
         <v>0</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
-      <c r="N19">
-        <v>1</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20">
-        <v>6</v>
-      </c>
-      <c r="C20">
-        <v>5</v>
-      </c>
-      <c r="D20">
-        <v>5</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>6</v>
-      </c>
-      <c r="J20">
-        <v>4</v>
-      </c>
-      <c r="K20">
-        <v>5</v>
       </c>
       <c r="L20">
         <v>3</v>
       </c>
       <c r="M20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20">
         <v>0</v>
       </c>
       <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>7</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>7</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <v>6</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21">
+        <v>3</v>
+      </c>
+      <c r="N21">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>2</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
         <v>19</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H31" t="s">
         <v>23</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E31" t="s">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
         <v>1</v>
       </c>
-      <c r="F31">
-        <f>B19+R2</f>
-        <v>7</v>
-      </c>
-      <c r="H31">
+      <c r="F32">
         <f>B20+S2</f>
         <v>6</v>
       </c>
-      <c r="I31">
-        <f>F31+H31</f>
-        <v>13</v>
-      </c>
-      <c r="N31" t="s">
-        <v>1</v>
-      </c>
-      <c r="O31" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E32" t="s">
+      <c r="H32">
+        <f>B21+T2</f>
+        <v>8</v>
+      </c>
+      <c r="I32">
+        <f>F32+H32</f>
+        <v>14</v>
+      </c>
+      <c r="O32" s="6"/>
+      <c r="Q32" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="R32" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
         <v>2</v>
       </c>
-      <c r="F32">
-        <f>C19+R3</f>
-        <v>8</v>
-      </c>
-      <c r="H32">
+      <c r="F33">
         <f>C20+S3</f>
-        <v>6</v>
-      </c>
-      <c r="I32">
-        <f t="shared" ref="I32:I45" si="0">F32+H32</f>
-        <v>14</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O32" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33">
+        <f>C21+T3</f>
+        <v>8</v>
+      </c>
+      <c r="I33">
+        <f t="shared" ref="I33:I46" si="0">F33+H33</f>
+        <v>15</v>
+      </c>
+      <c r="N33" s="2"/>
+      <c r="O33" s="6"/>
+      <c r="Q33" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R33" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
         <v>3</v>
       </c>
-      <c r="F33">
-        <f>D19+R4</f>
-        <v>7</v>
-      </c>
-      <c r="H33">
+      <c r="F34">
         <f>D20+S4</f>
         <v>6</v>
       </c>
-      <c r="I33">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O33" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E34" t="s">
-        <v>4</v>
-      </c>
-      <c r="F34">
-        <f>E19+R5</f>
-        <v>8</v>
-      </c>
       <c r="H34">
-        <f>E20+S5</f>
-        <v>4</v>
+        <f>D21+T4</f>
+        <v>8</v>
       </c>
       <c r="I34">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="N34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O34" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" s="2">
-        <f>F19+R6</f>
-        <v>8</v>
-      </c>
-      <c r="G35" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="N34" s="2"/>
+      <c r="O34" s="6"/>
+      <c r="Q34" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="R34" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35">
+        <f>E20+S5</f>
+        <v>7</v>
+      </c>
       <c r="H35">
-        <f>F20+S6</f>
-        <v>4</v>
+        <f>E21+T5</f>
+        <v>7</v>
       </c>
       <c r="I35">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="N35" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O35" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E36" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="2">
-        <f>H19+R8</f>
-        <v>8</v>
-      </c>
-      <c r="G36" s="2"/>
-      <c r="H36">
-        <f>H20+S8</f>
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="N35" s="2"/>
+      <c r="O35" s="6"/>
+      <c r="Q35" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="R35" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E36" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="6">
+        <f>F20+S6</f>
+        <v>8</v>
+      </c>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6">
+        <f>F21+T6</f>
+        <v>6</v>
       </c>
       <c r="I36">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="N36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O36" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E37" t="s">
-        <v>6</v>
-      </c>
-      <c r="F37">
-        <f>I19+R9</f>
-        <v>2</v>
-      </c>
-      <c r="H37">
-        <f>I20+S9</f>
+        <v>14</v>
+      </c>
+      <c r="N36" s="2"/>
+      <c r="O36" s="6"/>
+      <c r="Q36" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="R36" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E37" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="2">
+        <f>H20+S8</f>
         <v>11</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6">
+        <f>H21+T8</f>
+        <v>4</v>
       </c>
       <c r="I37">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="N37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O37" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E38" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38">
-        <f>J19+R10</f>
-        <v>4</v>
-      </c>
-      <c r="H38">
-        <f>J20+S10</f>
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="N37" s="2"/>
+      <c r="O37" s="6"/>
+      <c r="Q37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E38" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="6">
+        <f>I20+S9</f>
+        <v>2</v>
+      </c>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6">
+        <f>I21+T9</f>
+        <v>12</v>
       </c>
       <c r="I38">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O38" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F39">
-        <f>K19+R11</f>
-        <v>5</v>
-      </c>
-      <c r="H39">
-        <f>K20+S11</f>
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="N38" s="2"/>
+      <c r="O38" s="6"/>
+      <c r="Q38" t="s">
+        <v>4</v>
+      </c>
+      <c r="R38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="6">
+        <f>J20+S10</f>
+        <v>5</v>
+      </c>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6">
+        <f>J21+T10</f>
+        <v>10</v>
       </c>
       <c r="I39">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="N39" t="s">
-        <v>3</v>
-      </c>
-      <c r="O39" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E40" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40">
-        <f>L19+R12</f>
-        <v>7</v>
-      </c>
-      <c r="H40">
-        <f>L20+S12</f>
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="N39" s="2"/>
+      <c r="O39" s="6"/>
+      <c r="Q39" t="s">
+        <v>17</v>
+      </c>
+      <c r="R39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E40" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="6">
+        <f>K20+S11</f>
+        <v>4</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6">
+        <f>K21+T11</f>
+        <v>11</v>
       </c>
       <c r="I40">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="N40" t="s">
+        <v>15</v>
+      </c>
+      <c r="O40" s="6"/>
+      <c r="Q40" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="R40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E41" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="O40" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E41" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41">
-        <f>M19+R13</f>
-        <v>7</v>
-      </c>
-      <c r="H41">
-        <f>M20+S13</f>
-        <v>7</v>
+      <c r="F41" s="6">
+        <f>L20+S12</f>
+        <v>9</v>
+      </c>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6">
+        <f>L21+T12</f>
+        <v>6</v>
       </c>
       <c r="I41">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="N41" t="s">
+        <v>15</v>
+      </c>
+      <c r="O41" s="6"/>
+      <c r="Q41" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="O41" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E42" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42">
-        <f>N19+R14</f>
-        <v>6</v>
-      </c>
-      <c r="H42">
-        <f>N20+S14</f>
-        <v>7</v>
+      <c r="R41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="6">
+        <f>M20+S13</f>
+        <v>7</v>
+      </c>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6">
+        <f>M21+T13</f>
+        <v>8</v>
       </c>
       <c r="I42">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="N42" t="s">
+        <v>15</v>
+      </c>
+      <c r="O42" s="6"/>
+      <c r="Q42" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E43" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O42" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E43" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
+      <c r="F43" s="6">
+        <f>N20+S14</f>
+        <v>7</v>
+      </c>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6">
+        <f>N21+T14</f>
+        <v>7</v>
       </c>
       <c r="I43">
         <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="O43" s="6"/>
+      <c r="Q43" t="s">
+        <v>3</v>
+      </c>
+      <c r="R43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E44" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="6">
         <v>0</v>
       </c>
-      <c r="N43" t="s">
-        <v>8</v>
-      </c>
-      <c r="O43" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E44" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44">
-        <f>P19+R16</f>
-        <v>8</v>
-      </c>
-      <c r="H44">
-        <f>P20+S16</f>
-        <v>6</v>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6">
+        <v>0</v>
       </c>
       <c r="I44">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O44" s="6"/>
+      <c r="Q44" t="s">
         <v>14</v>
       </c>
-      <c r="N44" t="s">
-        <v>7</v>
-      </c>
-      <c r="O44" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E45" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F45" s="2">
-        <f>P19+R17</f>
-        <v>8</v>
-      </c>
-      <c r="G45" s="2"/>
-      <c r="H45">
-        <f>P20+S17</f>
-        <v>6</v>
+      <c r="R44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E45" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="6">
+        <f>P20+S16</f>
+        <v>8</v>
+      </c>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6">
+        <f>P21+T16</f>
+        <v>7</v>
       </c>
       <c r="I45">
         <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="O45" s="6"/>
+      <c r="Q45" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E46" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="6">
+        <f>P20+S17</f>
+        <v>8</v>
+      </c>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6">
+        <f>P21+T17</f>
+        <v>7</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="O46" s="6"/>
+      <c r="Q46" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E47" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" s="6">
+        <f>G20+S7</f>
+        <v>7</v>
+      </c>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6">
+        <f>G21+T7</f>
+        <v>7</v>
+      </c>
+      <c r="I47">
+        <f>F47+H47</f>
         <v>14</v>
       </c>
-      <c r="N45" t="s">
-        <v>6</v>
-      </c>
-      <c r="O45" s="6">
+      <c r="O47" s="6"/>
+      <c r="Q47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="R47">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E46" t="s">
-        <v>32</v>
-      </c>
-      <c r="F46">
-        <f>H19+R8</f>
-        <v>8</v>
-      </c>
-      <c r="H46">
-        <f>H20+S8</f>
-        <v>4</v>
-      </c>
-      <c r="N46" t="s">
+    <row r="48" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E48" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48" s="2">
+        <f>S18</f>
+        <v>15</v>
+      </c>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6">
+        <f>T18</f>
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <f>H48+F48</f>
+        <v>16</v>
+      </c>
+      <c r="Q48" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O46" s="6">
+      <c r="R48">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="N33:O46">
-    <sortCondition descending="1" ref="O31"/>
+  <sortState ref="Q32:R48">
+    <sortCondition descending="1" ref="R32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>